<commit_message>
Updates ITC/PTC naming in .mdl and WebAppData to mirror power sector naming system
</commit_message>
<xml_diff>
--- a/InputData/indst/IFTQfS/Indst Fuels Qualifying for Support.xlsx
+++ b/InputData/indst/IFTQfS/Indst Fuels Qualifying for Support.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\indst\IFTQfS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E804866A-622E-44A3-8C8C-469A3A17C7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26E8FDA-825D-45E0-9A1C-D179A264BAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61260" yWindow="1725" windowWidth="24900" windowHeight="14490" xr2:uid="{CEBBDD15-8244-44C2-A2EB-EB506D69E415}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{CEBBDD15-8244-44C2-A2EB-EB506D69E415}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="IFTQfS-PTC" sheetId="2" r:id="rId2"/>
-    <sheet name="IFTQfS-ITC" sheetId="3" r:id="rId3"/>
+    <sheet name="IFTQfS-production" sheetId="2" r:id="rId2"/>
+    <sheet name="IFTQfS-investment" sheetId="3" r:id="rId3"/>
     <sheet name="IFTQfS-loans" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -96,21 +96,9 @@
     <t>Boolean</t>
   </si>
   <si>
-    <t>IFTQfS Industrial Fuel Types Qualifying for ITC</t>
-  </si>
-  <si>
-    <t>IFTQfS Industrial Fuel Types Qualifying for PTC</t>
-  </si>
-  <si>
     <t>IFTQfS Industrial Fuel Types Qualifying for Loans</t>
   </si>
   <si>
-    <t>clean industrial heat ITC/subsidy policies (when used for industrial heating purposes),</t>
-  </si>
-  <si>
-    <t>This variable specifies which fuel types qualify for the clean industrial heat PTC,</t>
-  </si>
-  <si>
     <t xml:space="preserve">and low-interest government loans to reduce the cost of financing clean equipment. </t>
   </si>
   <si>
@@ -118,6 +106,18 @@
   </si>
   <si>
     <t>low carbon hydrogen if</t>
+  </si>
+  <si>
+    <t>IFTQfS Industrial Fuel Types Qualifying for Clean Heat Production Subsidy</t>
+  </si>
+  <si>
+    <t>IFTQfS Industrial Fuel Types Qualifying for Clean Heat Investment Subsidy</t>
+  </si>
+  <si>
+    <t>This variable specifies which fuel types qualify for the clean industrial heat production,</t>
+  </si>
+  <si>
+    <t>clean industrial heat investment policies (when used for industrial heating purposes),</t>
   </si>
 </sst>
 </file>
@@ -503,28 +503,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74327C6-C2CB-4CD6-A944-44D7EC17E747}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,44 +532,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -591,12 +591,12 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -604,7 +604,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -612,7 +612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -620,7 +620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -628,7 +628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -644,7 +644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -652,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -684,17 +684,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -712,16 +712,16 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -729,7 +729,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -737,7 +737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -753,7 +753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -761,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -769,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -777,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -793,7 +793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -801,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -809,17 +809,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -841,12 +841,12 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -854,7 +854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -862,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -870,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -886,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -910,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -918,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -926,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -934,17 +934,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>1</v>

</xml_diff>